<commit_message>
Agregada la tabla de datos buena
</commit_message>
<xml_diff>
--- a/src/Entrega2.xlsx
+++ b/src/Entrega2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agust\PycharmProjects\entrega-2\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicoh\OneDrive\Documentos\UBA\1ero-2020\Numerico\TPs\Entrega-3\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A362625-56ED-4D49-91C0-C6DCDE296784}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2DB51C-653A-41C8-A73E-82A80B88530F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{018AF0C9-1332-47C6-90FC-A18FAE2476D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{018AF0C9-1332-47C6-90FC-A18FAE2476D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -910,9 +910,6 @@
                 <c:pt idx="120">
                   <c:v>121</c:v>
                 </c:pt>
-                <c:pt idx="123">
-                  <c:v>7381</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1382,7 +1379,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-AR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1420,7 +1417,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="475762552"/>
@@ -1499,7 +1496,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-AR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1537,7 +1534,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="475762224"/>
@@ -1585,7 +1582,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2490,10 +2487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CD16D5C-3915-4797-AD42-A46A7196562F}">
-  <dimension ref="A1:T124"/>
+  <dimension ref="A1:T121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5963,12 +5960,6 @@
         <v>9.0894483128596429E-5</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D124" s="1">
-        <f>SUM(D1:D121)</f>
-        <v>7381</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>